<commit_message>
Site updated at: 2018-05-17 00:56:21 UTC
</commit_message>
<xml_diff>
--- a/class/seminar_fundamental_areas/data1/jinkou.xlsx
+++ b/class/seminar_fundamental_areas/data1/jinkou.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmuka\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33C397F-EB01-42DD-B849-794C83DEB957}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jinkou" sheetId="1" r:id="rId1"/>
@@ -132,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +294,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -475,7 +485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -590,6 +600,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -719,8 +744,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1077,22 +1114,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
@@ -1100,499 +1147,503 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1693</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>1647</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>3340</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>1315</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>2593</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>2431</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>5024</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>2086</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>1017</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1034</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>2051</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>876</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>171</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>173</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>344</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>171</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>200</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>371</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>1404</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>1381</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>2785</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>1073</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>898</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>924</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>1822</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>698</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>1929</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>2091</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>4020</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>1655</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>525</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>363</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>888</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>477</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>766</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>829</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>1595</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>614</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>337</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>347</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>684</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>4658</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>4930</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>9588</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>3831</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>496</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>534</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>1030</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>415</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>473</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>437</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>910</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>898</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>974</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>1872</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>738</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>1940</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>2063</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>4003</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>1570</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>1388</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>1386</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>2774</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>1212</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>1881</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>2029</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>3910</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>1559</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>3351</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>3520</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>6871</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>2604</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>2087</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>1972</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>4059</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>1818</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>3051</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>3091</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>6142</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>2323</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>3791</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>3919</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>7710</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>2883</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>2610</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>2637</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <v>5247</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <v>2051</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>973</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>992</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>1965</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <v>724</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>1183</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>1015</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <v>2198</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <v>998</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>2128</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>2129</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="3">
         <v>4257</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <v>1666</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>2318</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>2034</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="3">
         <v>4352</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>1883</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>44730</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>45082</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="3">
         <v>89812</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <v>36070</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>